<commit_message>
Student Option uploading result done
</commit_message>
<xml_diff>
--- a/scripts/01_IAT_IJSO_KOTA_07-05-2017.xlsx
+++ b/scripts/01_IAT_IJSO_KOTA_07-05-2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="15360"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="13540"/>
   </bookViews>
   <sheets>
     <sheet name="ABCD" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3481" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3479" uniqueCount="131">
   <si>
     <t>ROLL NO</t>
   </si>
@@ -302,9 +302,6 @@
     <t>16435275</t>
   </si>
   <si>
-    <t>ADESH KUMAR</t>
-  </si>
-  <si>
     <t>15435144</t>
   </si>
   <si>
@@ -405,9 +402,6 @@
   </si>
   <si>
     <t>16435066</t>
-  </si>
-  <si>
-    <t>DEVANSH</t>
   </si>
   <si>
     <t>16405441</t>
@@ -802,9 +796,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9.3984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
@@ -1569,8 +1568,8 @@
       </c>
     </row>
     <row r="4" spans="1:84" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>91</v>
+      <c r="A4">
+        <v>15435143</v>
       </c>
       <c r="B4">
         <v>9</v>
@@ -1824,7 +1823,7 @@
     </row>
     <row r="5" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5">
         <v>9</v>
@@ -2078,7 +2077,7 @@
     </row>
     <row r="6" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -2323,7 +2322,7 @@
     </row>
     <row r="7" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7">
         <v>9</v>
@@ -2353,7 +2352,7 @@
         <v>88</v>
       </c>
       <c r="K7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L7" t="s">
         <v>85</v>
@@ -2577,7 +2576,7 @@
     </row>
     <row r="8" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -2831,7 +2830,7 @@
     </row>
     <row r="9" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9">
         <v>9</v>
@@ -3085,7 +3084,7 @@
     </row>
     <row r="10" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -3339,7 +3338,7 @@
     </row>
     <row r="11" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -3593,7 +3592,7 @@
     </row>
     <row r="12" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -3824,7 +3823,7 @@
         <v>88</v>
       </c>
       <c r="BZ12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="CA12" t="s">
         <v>87</v>
@@ -3847,7 +3846,7 @@
     </row>
     <row r="13" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B13">
         <v>9</v>
@@ -4101,7 +4100,7 @@
     </row>
     <row r="14" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -4355,7 +4354,7 @@
     </row>
     <row r="15" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15">
         <v>9</v>
@@ -4609,7 +4608,7 @@
     </row>
     <row r="16" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B16">
         <v>9</v>
@@ -4863,7 +4862,7 @@
     </row>
     <row r="17" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B17">
         <v>10</v>
@@ -5117,7 +5116,7 @@
     </row>
     <row r="18" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B18">
         <v>9</v>
@@ -5371,7 +5370,7 @@
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B19">
         <v>9</v>
@@ -5625,7 +5624,7 @@
     </row>
     <row r="20" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20">
         <v>9</v>
@@ -5879,7 +5878,7 @@
     </row>
     <row r="21" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B21">
         <v>9</v>
@@ -6133,7 +6132,7 @@
     </row>
     <row r="22" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22">
         <v>10</v>
@@ -6387,7 +6386,7 @@
     </row>
     <row r="23" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23">
         <v>9</v>
@@ -6608,7 +6607,7 @@
     </row>
     <row r="24" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B24">
         <v>9</v>
@@ -6862,7 +6861,7 @@
     </row>
     <row r="25" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B25">
         <v>9</v>
@@ -7116,7 +7115,7 @@
     </row>
     <row r="26" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B26">
         <v>9</v>
@@ -7370,7 +7369,7 @@
     </row>
     <row r="27" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B27">
         <v>9</v>
@@ -7624,7 +7623,7 @@
     </row>
     <row r="28" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B28">
         <v>10</v>
@@ -7878,7 +7877,7 @@
     </row>
     <row r="29" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B29">
         <v>9</v>
@@ -8132,7 +8131,7 @@
     </row>
     <row r="30" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B30">
         <v>10</v>
@@ -8386,7 +8385,7 @@
     </row>
     <row r="31" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B31">
         <v>9</v>
@@ -8640,7 +8639,7 @@
     </row>
     <row r="32" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B32">
         <v>9</v>
@@ -8894,7 +8893,7 @@
     </row>
     <row r="33" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B33">
         <v>9</v>
@@ -9148,7 +9147,7 @@
     </row>
     <row r="34" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B34">
         <v>10</v>
@@ -9399,7 +9398,7 @@
     </row>
     <row r="35" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B35">
         <v>9</v>
@@ -9644,7 +9643,7 @@
     </row>
     <row r="36" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B36">
         <v>10</v>
@@ -9897,8 +9896,8 @@
       </c>
     </row>
     <row r="37" spans="1:84" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
-        <v>126</v>
+      <c r="A37">
+        <v>16405440</v>
       </c>
       <c r="B37">
         <v>9</v>
@@ -10152,7 +10151,7 @@
     </row>
     <row r="38" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B38">
         <v>10</v>
@@ -10406,7 +10405,7 @@
     </row>
     <row r="39" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B39">
         <v>9</v>
@@ -10660,7 +10659,7 @@
     </row>
     <row r="40" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B40">
         <v>9</v>
@@ -10914,7 +10913,7 @@
     </row>
     <row r="41" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B41">
         <v>10</v>
@@ -11168,7 +11167,7 @@
     </row>
     <row r="42" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B42">
         <v>9</v>
@@ -11335,7 +11334,7 @@
     </row>
     <row r="43" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B43">
         <v>9</v>

</xml_diff>